<commit_message>
Updating Excel Support Materials
</commit_message>
<xml_diff>
--- a/.Excel/AdvancedCurveFeatures.xlsx
+++ b/.Excel/AdvancedCurveFeatures.xlsx
@@ -1,26 +1,168 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BOOK\.SWAPS_BOOK\.Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6F63CF-019D-4678-9148-F4A785A38F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7500"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="38700" windowHeight="17370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Curve Jacobian" sheetId="4" r:id="rId1"/>
+    <sheet name="ToYs" sheetId="1" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="dt">Sheet1!$J$4</definedName>
-    <definedName name="rate">Sheet1!$J$3</definedName>
+    <definedName name="AccruedInterestTotalPV">#REF!</definedName>
+    <definedName name="AnalyticalDV01">[2]Swaps!$C$68</definedName>
+    <definedName name="Annuity_Fixed">[2]Swaps!$C$61</definedName>
+    <definedName name="Annuity1">'[1]XCCY Calculator'!$C$32</definedName>
+    <definedName name="Annuity2">'[1]XCCY Calculator'!$D$32</definedName>
+    <definedName name="ApplyBump">[2]Swaps!$C$71</definedName>
+    <definedName name="Approximate">[2]Swaps!$C$14</definedName>
+    <definedName name="AsOfDate">[2]Settings!$C$3</definedName>
+    <definedName name="BumpSize">'[2]Discount Factors'!$C$5</definedName>
+    <definedName name="BumpSizeLiborRates">'[2]Libor Rates'!$C$4</definedName>
+    <definedName name="CSACurrency">'[1]XCCY Calculator'!$C$11</definedName>
+    <definedName name="Currency">[2]Swaps!$C$6</definedName>
+    <definedName name="DayCountBasis1">'[1]XCCY Calculator'!$C$24</definedName>
+    <definedName name="DayCountBasis2">'[1]XCCY Calculator'!$D$24</definedName>
+    <definedName name="DiscountCurve">[2]Swaps!$C$30</definedName>
+    <definedName name="DiscountFactor1Y">'[3]Bootrapping USD3ML'!$F$11</definedName>
+    <definedName name="DiscountFactor2Y">'[3]Bootrapping USD3ML'!$F$12</definedName>
+    <definedName name="DiscountFactor3Y">'[3]Bootrapping USD3ML'!$F$13</definedName>
+    <definedName name="DiscountFactor4Y">'[3]Bootrapping USD3ML'!$F$14</definedName>
+    <definedName name="DiscountFactor5Y">'[3]Bootrapping USD3ML'!$F$15</definedName>
+    <definedName name="dt">ToYs!$J$4</definedName>
+    <definedName name="DurationFixed">[2]Swaps!$C$65</definedName>
+    <definedName name="DurationFloat">[2]Swaps!$C$66</definedName>
+    <definedName name="EURIBOR3M">'[1]XCCY Calculator'!$Y$6:$Z$49</definedName>
+    <definedName name="FixedLegFrequencySelected">[2]Swaps!$C$42</definedName>
+    <definedName name="FloatLegFrequencySelected">[2]Swaps!$C$47</definedName>
+    <definedName name="ForecastCurve">[2]Swaps!$C$29</definedName>
+    <definedName name="FORWARDFX">'[1]XCCY Calculator'!$AE$6:$AF$49</definedName>
+    <definedName name="Frequency">#REF!</definedName>
+    <definedName name="HazardRate">#REF!</definedName>
+    <definedName name="LegCurrency1">'[1]XCCY Calculator'!$C$14</definedName>
+    <definedName name="LegCurrency2">'[1]XCCY Calculator'!$D$14</definedName>
+    <definedName name="LegNotional1">'[1]XCCY Calculator'!$C$15</definedName>
+    <definedName name="LegNotional2">'[1]XCCY Calculator'!$D$15</definedName>
+    <definedName name="LegPV1">'[1]XCCY Calculator'!$C$28</definedName>
+    <definedName name="LegPV2">'[1]XCCY Calculator'!$D$28</definedName>
+    <definedName name="LegPVNoSpread1">'[1]XCCY Calculator'!$C$30</definedName>
+    <definedName name="LegPVNoSpread2">'[1]XCCY Calculator'!$D$30</definedName>
+    <definedName name="LegResetsRequired1">'[1]XCCY Calculator'!$C$21</definedName>
+    <definedName name="LegResetsRequired2">'[1]XCCY Calculator'!$D$21</definedName>
+    <definedName name="LegSpotFX1">'[1]XCCY Calculator'!$C$22</definedName>
+    <definedName name="LegSpotFX2">'[1]XCCY Calculator'!$D$22</definedName>
+    <definedName name="LegType1">'[1]XCCY Calculator'!$C$17</definedName>
+    <definedName name="LegType2">'[1]XCCY Calculator'!$D$17</definedName>
+    <definedName name="Maturity">#REF!</definedName>
+    <definedName name="MaturityDate">'[1]XCCY Calculator'!$C$5</definedName>
+    <definedName name="MaturityYears">'[1]XCCY Calculator'!$D$5</definedName>
+    <definedName name="MTM">'[1]XCCY Calculator'!$C$8</definedName>
+    <definedName name="N">[2]Swaps!$C$7</definedName>
+    <definedName name="Notional">#REF!</definedName>
+    <definedName name="NotionalExchanges">'[1]XCCY Calculator'!$C$9</definedName>
+    <definedName name="NotionalExchanges1">'[1]XCCY Calculator'!$C$31</definedName>
+    <definedName name="NotionalExchanges2">'[1]XCCY Calculator'!$D$31</definedName>
+    <definedName name="NumericalDV01">[2]Swaps!$C$74</definedName>
+    <definedName name="OverrideMarketFrequency">[2]Swaps!$C$38</definedName>
+    <definedName name="p">[2]Swaps!$C$56</definedName>
+    <definedName name="ParRate1Y">'[3]Bootrapping USD3ML'!$E$11</definedName>
+    <definedName name="ParRate2Y">'[3]Bootrapping USD3ML'!$E$12</definedName>
+    <definedName name="ParRate3Y">'[3]Bootrapping USD3ML'!$E$13</definedName>
+    <definedName name="ParRate4Y">'[3]Bootrapping USD3ML'!$E$14</definedName>
+    <definedName name="ParRate5Y">'[3]Bootrapping USD3ML'!$E$15</definedName>
+    <definedName name="PayReceive1">'[1]XCCY Calculator'!$C$16</definedName>
+    <definedName name="PayReceive2">'[1]XCCY Calculator'!$D$16</definedName>
+    <definedName name="Periodicity">'[2]Discount Factors'!$C$4</definedName>
+    <definedName name="Phi">#REF!</definedName>
+    <definedName name="Premium">#REF!</definedName>
+    <definedName name="PremiumLegTotalPV">#REF!</definedName>
+    <definedName name="ProtectionLegTotalPV">#REF!</definedName>
+    <definedName name="PV_FixedLeg">[2]Swaps!$C$52</definedName>
+    <definedName name="PV_FloatLeg">[2]Swaps!$C$53</definedName>
+    <definedName name="PV_FloatSpread">[2]Swaps!$C$54</definedName>
+    <definedName name="PV_Swap">[2]Swaps!$C$55</definedName>
+    <definedName name="PV01_">[2]Swaps!$C$67</definedName>
+    <definedName name="PVlets_Fixed">[2]Swaps!$M$6:$M$55</definedName>
+    <definedName name="PVlets_Float">[2]Swaps!$AA$6:$AA$55</definedName>
+    <definedName name="r_fixed">[2]Swaps!$C$8</definedName>
+    <definedName name="rate">ToYs!$J$3</definedName>
+    <definedName name="RateOrSpread1">'[1]XCCY Calculator'!$C$18</definedName>
+    <definedName name="RateOrSpread2">'[1]XCCY Calculator'!$D$18</definedName>
+    <definedName name="RecoveryRate">#REF!</definedName>
+    <definedName name="ResetCurrency">'[1]XCCY Calculator'!$C$10</definedName>
+    <definedName name="s">[2]Swaps!$C$11</definedName>
+    <definedName name="SetDiscFactToOne">[2]Swaps!$C$31</definedName>
+    <definedName name="Settings.COB">[4]Settings!$B$3</definedName>
+    <definedName name="SpotFX">'[1]XCCY Calculator'!$AF$6</definedName>
+    <definedName name="T">[2]Swaps!$C$12</definedName>
+    <definedName name="t_i">[2]Swaps!$C$43</definedName>
+    <definedName name="t_j">[2]Swaps!$C$48</definedName>
+    <definedName name="TradeCurrency">'[1]XCCY Calculator'!$C$7</definedName>
+    <definedName name="TradeNotional">'[1]XCCY Calculator'!$C$6</definedName>
+    <definedName name="USD_SOFR_CURVE_GENERATOR">[4]Settings!$I$5</definedName>
+    <definedName name="USD_SOFR_SWAP_GENERATOR">[4]Settings!$N$5</definedName>
+    <definedName name="USDLIBOR3M">'[1]XCCY Calculator'!$AB$6:$AC$49</definedName>
+    <definedName name="ValuationCurrency">'[1]XCCY Calculator'!$C$12</definedName>
+    <definedName name="ValuationFXAdj1">'[1]XCCY Calculator'!$C$23</definedName>
+    <definedName name="ValuationFXAdj2">'[1]XCCY Calculator'!$D$23</definedName>
+    <definedName name="YearFraction">#REF!</definedName>
+    <definedName name="ZeroRate">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029" calcMode="manual" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>P(t,T)</t>
   </si>
@@ -74,17 +216,714 @@
   <si>
     <t>Curve Inputs</t>
   </si>
+  <si>
+    <t>Ultra-Fast Yield Curves using Inverse Jacobian</t>
+  </si>
+  <si>
+    <t>New Forwards</t>
+  </si>
+  <si>
+    <t>New Fwds</t>
+  </si>
+  <si>
+    <t>Original Fwds</t>
+  </si>
+  <si>
+    <t>Chg in Mkt Data</t>
+  </si>
+  <si>
+    <t>Chg in Forwards</t>
+  </si>
+  <si>
+    <t>From Calibration</t>
+  </si>
+  <si>
+    <t>From Jacobian</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>NEW</t>
+    </r>
+  </si>
+  <si>
+    <t>+/-</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OLD</t>
+    </r>
+  </si>
+  <si>
+    <t>dP (%)</t>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>1Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>2Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>3Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>4Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>5Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>1Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>2Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>3Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>4Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>5Y</t>
+    </r>
+  </si>
+  <si>
+    <t>dL</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>1Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OIS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>1Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>2Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OIS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>2Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>3Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OIS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>3Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>4Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OIS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>4Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>5Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OIS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OIS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>5Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>1Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>IRS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>1Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>2Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>IRS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>2Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>3Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>IRS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>3Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>4Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>IRS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>4Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>5Y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>IRS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IRS</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="22"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>5Y</t>
+    </r>
+  </si>
+  <si>
+    <t>Use Jacobian to Imply Change in Forward Rates</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="26"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>NEW</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="26"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="26"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OLD</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="26"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + dL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Change in Forwards = J</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="26"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>.dP = (dL/dP).dP = dL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Inverse Jacobian, J</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="26"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (or dL/dP)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.00000%"/>
+    <numFmt numFmtId="168" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,8 +945,125 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="22"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="22"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="22"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="22"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="22"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="22"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="26"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="26"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="26"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="26"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,8 +1076,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -129,11 +1091,331 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -144,7 +1426,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -159,14 +1441,185 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -183,14 +1636,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -254,7 +1710,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$37</c:f>
+              <c:f>ToYs!$C$8:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="30"/>
@@ -353,7 +1809,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$8:$F$37</c:f>
+              <c:f>ToYs!$F$8:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="30"/>
@@ -376,22 +1832,22 @@
                   <c:v>9.9999999999999655E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7499999999999988E-2</c:v>
+                  <c:v>9.9999999999999881E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9999999999999204E-3</c:v>
+                  <c:v>1.7499999999999918E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>9.9999999999999672E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2500000000000018E-2</c:v>
+                  <c:v>1.0000000000000018E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9.9999999999999915E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.9999999999999915E-3</c:v>
+                  <c:v>1.2499999999999992E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>9.9999999999999464E-3</c:v>
@@ -451,6 +1907,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-68A2-4945-92AB-BBFCB28159FD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -463,7 +1924,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$37</c:f>
+              <c:f>ToYs!$C$8:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="30"/>
@@ -562,7 +2023,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$8:$E$37</c:f>
+              <c:f>ToYs!$E$8:$E$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="30"/>
@@ -660,6 +2121,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-68A2-4945-92AB-BBFCB28159FD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -669,7 +2135,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="220383488"/>
         <c:axId val="136642944"/>
@@ -774,7 +2239,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -790,6 +2261,841 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="IR Markets"/>
+      <sheetName val="IRS Conventions"/>
+      <sheetName val="UST Spread"/>
+      <sheetName val="IRS Contract"/>
+      <sheetName val="IR Scenarios"/>
+      <sheetName val="IRS Example"/>
+      <sheetName val="IBOR vs OIS Fixings"/>
+      <sheetName val="IRS Pricing"/>
+      <sheetName val="IRS Pricing2"/>
+      <sheetName val="IRS Pricing3"/>
+      <sheetName val="IRS Pricing Case Study"/>
+      <sheetName val="IRS Risk"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="CDS Diagram"/>
+      <sheetName val="CDS Cash Flows"/>
+      <sheetName val="CDS Legs"/>
+      <sheetName val="FX Forward Replication"/>
+      <sheetName val="XCCY Cash Flows"/>
+      <sheetName val="XCCY Booking"/>
+      <sheetName val="XCCY Features"/>
+      <sheetName val="XCCY Calculator"/>
+      <sheetName val="Forward Rate Formula"/>
+      <sheetName val="Interpolation"/>
+      <sheetName val="Curve Dependencies"/>
+      <sheetName val="Bootstrapping Problem"/>
+      <sheetName val="Curve Jacobian"/>
+      <sheetName val="Risk Jacobian"/>
+      <sheetName val="SOFR Curve"/>
+      <sheetName val="SOFR Basis"/>
+      <sheetName val="DV01 Risk"/>
+      <sheetName val="Jacobian Transformations"/>
+      <sheetName val="Asset Swap"/>
+      <sheetName val="Asset Swap Diagrams"/>
+      <sheetName val="Asset Swap Cash Flows"/>
+      <sheetName val="ASW Initial Exchanges"/>
+      <sheetName val="ASW Coupons"/>
+      <sheetName val="ASW Final Exchanges"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20">
+        <row r="5">
+          <cell r="C5" t="e">
+            <v>#NAME?</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>1Y</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6">
+            <v>1000000</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7" t="str">
+            <v>USD</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8" t="str">
+            <v>YES</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="C9" t="str">
+            <v>YES</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="C10" t="str">
+            <v>NO</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12" t="e">
+            <v>#REF!</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14" t="e">
+            <v>#REF!</v>
+          </cell>
+          <cell r="D14" t="e">
+            <v>#NAME?</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="C15" t="e">
+            <v>#REF!</v>
+          </cell>
+          <cell r="D15" t="e">
+            <v>#REF!</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="C16" t="e">
+            <v>#NAME?</v>
+          </cell>
+          <cell r="D16" t="e">
+            <v>#NAME?</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="C17" t="e">
+            <v>#REF!</v>
+          </cell>
+          <cell r="D17" t="e">
+            <v>#REF!</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="C18" t="e">
+            <v>#NAME?</v>
+          </cell>
+          <cell r="D18" t="e">
+            <v>#NAME?</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>-1921.2846162773203</v>
+          </cell>
+          <cell r="D28" t="str">
+            <v>USD</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32" t="str">
+            <v>EUR</v>
+          </cell>
+          <cell r="D32" t="str">
+            <v>USD</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Settings"/>
+      <sheetName val="Discount Factors"/>
+      <sheetName val="Libor Rates"/>
+      <sheetName val="Swaps"/>
+      <sheetName val="Case Study"/>
+      <sheetName val="Cashflow Diagrams"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="C3">
+            <v>44760</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="4">
+          <cell r="C4">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5">
+            <v>-1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="4">
+          <cell r="C4">
+            <v>-1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="6">
+          <cell r="C6" t="str">
+            <v>EUR</v>
+          </cell>
+          <cell r="M6">
+            <v>10041.318001175765</v>
+          </cell>
+          <cell r="AA6">
+            <v>244.13666038522976</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>1000000</v>
+          </cell>
+          <cell r="M7">
+            <v>10069.279978978393</v>
+          </cell>
+          <cell r="AA7">
+            <v>545.91188130375895</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>0.01</v>
+          </cell>
+          <cell r="M8">
+            <v>10083.773610910694</v>
+          </cell>
+          <cell r="AA8">
+            <v>948.85052648010799</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="M9">
+            <v>10083.773610910694</v>
+          </cell>
+          <cell r="AA9">
+            <v>1252.2816762751261</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="M10">
+            <v>10069.279978978393</v>
+          </cell>
+          <cell r="AA10">
+            <v>1656.6860616269923</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+          <cell r="M11" t="str">
+            <v/>
+          </cell>
+          <cell r="AA11">
+            <v>2060.7860882409327</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>5</v>
+          </cell>
+          <cell r="M12" t="str">
+            <v/>
+          </cell>
+          <cell r="AA12">
+            <v>2363.8173367451723</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="M13" t="str">
+            <v/>
+          </cell>
+          <cell r="AA13">
+            <v>2766.6502410046801</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="M14" t="str">
+            <v/>
+          </cell>
+          <cell r="AA14">
+            <v>3168.5684950582686</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="M15" t="str">
+            <v/>
+          </cell>
+          <cell r="AA15">
+            <v>3467.5232716503706</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="M16" t="str">
+            <v/>
+          </cell>
+          <cell r="AA16" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="M17" t="str">
+            <v/>
+          </cell>
+          <cell r="AA17" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="M18" t="str">
+            <v/>
+          </cell>
+          <cell r="AA18" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="M19" t="str">
+            <v/>
+          </cell>
+          <cell r="AA19" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="M20" t="str">
+            <v/>
+          </cell>
+          <cell r="AA20" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="M21" t="str">
+            <v/>
+          </cell>
+          <cell r="AA21" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="M22" t="str">
+            <v/>
+          </cell>
+          <cell r="AA22" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="M23" t="str">
+            <v/>
+          </cell>
+          <cell r="AA23" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="M24" t="str">
+            <v/>
+          </cell>
+          <cell r="AA24" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="M25" t="str">
+            <v/>
+          </cell>
+          <cell r="AA25" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="M26" t="str">
+            <v/>
+          </cell>
+          <cell r="AA26" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="M27" t="str">
+            <v/>
+          </cell>
+          <cell r="AA27" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="M28" t="str">
+            <v/>
+          </cell>
+          <cell r="AA28" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29" t="str">
+            <v>EUR6ML</v>
+          </cell>
+          <cell r="M29" t="str">
+            <v/>
+          </cell>
+          <cell r="AA29" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>EURDiscFact</v>
+          </cell>
+          <cell r="M30" t="str">
+            <v/>
+          </cell>
+          <cell r="AA30" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="M31" t="str">
+            <v/>
+          </cell>
+          <cell r="AA31" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="M32" t="str">
+            <v/>
+          </cell>
+          <cell r="AA32" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="M33" t="str">
+            <v/>
+          </cell>
+          <cell r="AA33" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="M34" t="str">
+            <v/>
+          </cell>
+          <cell r="AA34" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="M35" t="str">
+            <v/>
+          </cell>
+          <cell r="AA35" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="M36" t="str">
+            <v/>
+          </cell>
+          <cell r="AA36" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="M37" t="str">
+            <v/>
+          </cell>
+          <cell r="AA37" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38" t="b">
+            <v>0</v>
+          </cell>
+          <cell r="M38" t="str">
+            <v/>
+          </cell>
+          <cell r="AA38" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="M39" t="str">
+            <v/>
+          </cell>
+          <cell r="AA39" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="M40" t="str">
+            <v/>
+          </cell>
+          <cell r="AA40" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="M41" t="str">
+            <v/>
+          </cell>
+          <cell r="AA41" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="C42" t="str">
+            <v>ANNUAL</v>
+          </cell>
+          <cell r="M42" t="str">
+            <v/>
+          </cell>
+          <cell r="AA42" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="C43">
+            <v>1</v>
+          </cell>
+          <cell r="M43" t="str">
+            <v/>
+          </cell>
+          <cell r="AA43" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="M44" t="str">
+            <v/>
+          </cell>
+          <cell r="AA44" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="M45" t="str">
+            <v/>
+          </cell>
+          <cell r="AA45" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="M46" t="str">
+            <v/>
+          </cell>
+          <cell r="AA46" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="C47" t="str">
+            <v>SEMI-ANNUAL</v>
+          </cell>
+          <cell r="M47" t="str">
+            <v/>
+          </cell>
+          <cell r="AA47" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="C48">
+            <v>0.5</v>
+          </cell>
+          <cell r="M48" t="str">
+            <v/>
+          </cell>
+          <cell r="AA48" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="M49" t="str">
+            <v/>
+          </cell>
+          <cell r="AA49" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="M50" t="str">
+            <v/>
+          </cell>
+          <cell r="AA50" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="M51" t="str">
+            <v/>
+          </cell>
+          <cell r="AA51" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="C52">
+            <v>50347.425180953942</v>
+          </cell>
+          <cell r="M52" t="str">
+            <v/>
+          </cell>
+          <cell r="AA52" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="C53">
+            <v>-18475.21223877064</v>
+          </cell>
+          <cell r="M53" t="str">
+            <v/>
+          </cell>
+          <cell r="AA53" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="C54">
+            <v>0</v>
+          </cell>
+          <cell r="M54" t="str">
+            <v/>
+          </cell>
+          <cell r="AA54" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="C55">
+            <v>31872.212942183301</v>
+          </cell>
+          <cell r="M55" t="str">
+            <v/>
+          </cell>
+          <cell r="AA55" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="C56">
+            <v>3.6695446037942926E-3</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="C61">
+            <v>5034742.5180953937</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="C65">
+            <v>3.0124123995007284</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="C66">
+            <v>3.5776417495404544</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="C67">
+            <v>503.47425180953934</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="C68">
+            <v>513.07547675619548</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="C71" t="b">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="C74">
+            <v>512.12530313245225</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Risk-Free Rates"/>
+      <sheetName val="Swap Pricing"/>
+      <sheetName val="USD Instruments &amp; Statistics"/>
+      <sheetName val="Interpolation"/>
+      <sheetName val="Bootrapping USD3ML"/>
+      <sheetName val="Solving USD3ML"/>
+      <sheetName val="Solving EUR3ML"/>
+      <sheetName val="Single Curve Calibration"/>
+      <sheetName val="Global Curve Calibration"/>
+      <sheetName val="USD LIBOR"/>
+      <sheetName val="USD SOFR Spikes"/>
+      <sheetName val="USD SOFR"/>
+      <sheetName val="USD SOFR BASIC vs ADVANCED"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="11">
+          <cell r="E11">
+            <v>1.7891899999999999E-2</v>
+          </cell>
+          <cell r="F11">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="E12">
+            <v>1.45947E-2</v>
+          </cell>
+          <cell r="F12">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13">
+            <v>1.5193E-2</v>
+          </cell>
+          <cell r="F13">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="E14">
+            <v>1.6036000000000002E-2</v>
+          </cell>
+          <cell r="F14">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="E15">
+            <v>1.6587999999999999E-2</v>
+          </cell>
+          <cell r="F15">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Settings"/>
+      <sheetName val="USD_SOFR_CURVE"/>
+      <sheetName val="USD_CURVE_DISPLAY"/>
+      <sheetName val="USD_SOFR_SWAPS"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="B3">
+            <v>44838</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="I5" t="str">
+            <v>USD_SOFR_CURVE:2</v>
+          </cell>
+          <cell r="N5" t="str">
+            <v>USD_SOFR_SWAP_TEMPLATE:1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -835,7 +3141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -868,9 +3174,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -903,6 +3226,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1078,10 +3418,920 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200DC679-5103-4F66-A4D6-DED6D755C2DF}">
+  <dimension ref="A2:AC28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="27" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="2" max="2" width="20.7109375" style="12" customWidth="1"/>
+    <col min="3" max="4" width="16.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="13" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="12" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="13" customWidth="1"/>
+    <col min="12" max="21" width="10.7109375" style="12" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" style="13" customWidth="1"/>
+    <col min="23" max="23" width="16.7109375" style="12" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="F2" s="63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="39.75" x14ac:dyDescent="0.35">
+      <c r="F3" s="62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="30" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="67"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="68"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="72" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="30" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="68"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="68"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="72"/>
+    </row>
+    <row r="8" spans="1:29" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="C8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="T8" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="U8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="W8" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="20">
+        <v>1.4459099999999999E-2</v>
+      </c>
+      <c r="D9" s="21">
+        <f t="shared" ref="D9:D18" ca="1" si="0">F9-C9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="23" cm="1">
+        <f t="array" aca="1" ref="F9:F18" ca="1">H9:H18+MMULT(L9:U18,J9:J18)</f>
+        <v>1.4459099999999999E-2</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="26">
+        <v>1.43591E-2</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="27">
+        <v>1E-4</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="28">
+        <v>1</v>
+      </c>
+      <c r="M9" s="29">
+        <v>0</v>
+      </c>
+      <c r="N9" s="29">
+        <v>0</v>
+      </c>
+      <c r="O9" s="29">
+        <v>0</v>
+      </c>
+      <c r="P9" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="29">
+        <v>0</v>
+      </c>
+      <c r="R9" s="29">
+        <v>0</v>
+      </c>
+      <c r="S9" s="29">
+        <v>0</v>
+      </c>
+      <c r="T9" s="29">
+        <v>0</v>
+      </c>
+      <c r="U9" s="31">
+        <v>0</v>
+      </c>
+      <c r="V9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="W9" s="32" cm="1">
+        <f t="array" aca="1" ref="W9:W18" ca="1">MMULT(L9:U18,J9:J18)</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="35">
+        <v>1.2432208400524256E-2</v>
+      </c>
+      <c r="D10" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0193365892335882E-7</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="24">
+        <f ca="1"/>
+        <v>1.243231033418318E-2</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="36">
+        <v>1.233231033418318E-2</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="38">
+        <v>-1.013100581860171</v>
+      </c>
+      <c r="M10" s="39">
+        <v>2.0131005818601713</v>
+      </c>
+      <c r="N10" s="39">
+        <v>0</v>
+      </c>
+      <c r="O10" s="39">
+        <v>0</v>
+      </c>
+      <c r="P10" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="39">
+        <v>0</v>
+      </c>
+      <c r="R10" s="39">
+        <v>0</v>
+      </c>
+      <c r="S10" s="39">
+        <v>0</v>
+      </c>
+      <c r="T10" s="39">
+        <v>0</v>
+      </c>
+      <c r="U10" s="41">
+        <v>0</v>
+      </c>
+      <c r="V10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="W10" s="33">
+        <f ca="1"/>
+        <v>1.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="35">
+        <v>1.2610652805549894E-2</v>
+      </c>
+      <c r="D11" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.4800618159464047E-8</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="24">
+        <f ca="1"/>
+        <v>1.2610737606168054E-2</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="36">
+        <v>1.2510737606168054E-2</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="38">
+        <v>1.6865017081063214E-16</v>
+      </c>
+      <c r="M11" s="39">
+        <v>-2.0381313856749337</v>
+      </c>
+      <c r="N11" s="39">
+        <v>3.0381313856749337</v>
+      </c>
+      <c r="O11" s="39">
+        <v>0</v>
+      </c>
+      <c r="P11" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="39">
+        <v>0</v>
+      </c>
+      <c r="R11" s="39">
+        <v>0</v>
+      </c>
+      <c r="S11" s="39">
+        <v>0</v>
+      </c>
+      <c r="T11" s="39">
+        <v>0</v>
+      </c>
+      <c r="U11" s="41">
+        <v>0</v>
+      </c>
+      <c r="V11" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="W11" s="33">
+        <f ca="1"/>
+        <v>1.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="35">
+        <v>1.3013010883558614E-2</v>
+      </c>
+      <c r="D12" s="43">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.458116442165259E-8</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="24">
+        <f ca="1"/>
+        <v>1.3013035464723035E-2</v>
+      </c>
+      <c r="G12" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="36">
+        <v>1.2913035464723036E-2</v>
+      </c>
+      <c r="I12" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="K12" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="38">
+        <v>5.5511151231257852E-17</v>
+      </c>
+      <c r="M12" s="39">
+        <v>0</v>
+      </c>
+      <c r="N12" s="39">
+        <v>-3.0769983737932272</v>
+      </c>
+      <c r="O12" s="39">
+        <v>4.0769983737932272</v>
+      </c>
+      <c r="P12" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="39">
+        <v>0</v>
+      </c>
+      <c r="R12" s="39">
+        <v>0</v>
+      </c>
+      <c r="S12" s="39">
+        <v>0</v>
+      </c>
+      <c r="T12" s="39">
+        <v>0</v>
+      </c>
+      <c r="U12" s="41">
+        <v>0</v>
+      </c>
+      <c r="V12" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="W12" s="33">
+        <f ca="1"/>
+        <v>1.0000000000000005E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="35">
+        <v>1.4078369265823502E-2</v>
+      </c>
+      <c r="D13" s="43">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1.9093539810333127E-7</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="24">
+        <f ca="1"/>
+        <v>1.4078178330425399E-2</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="36">
+        <v>1.39781783304254E-2</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="K13" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="45">
+        <v>-2.2935090300213447E-16</v>
+      </c>
+      <c r="M13" s="46">
+        <v>5.697241084667845E-16</v>
+      </c>
+      <c r="N13" s="46">
+        <v>-5.697241084667845E-16</v>
+      </c>
+      <c r="O13" s="46">
+        <v>-4.1316185651899975</v>
+      </c>
+      <c r="P13" s="47">
+        <v>5.1316185651899975</v>
+      </c>
+      <c r="Q13" s="39">
+        <v>0</v>
+      </c>
+      <c r="R13" s="39">
+        <v>0</v>
+      </c>
+      <c r="S13" s="39">
+        <v>0</v>
+      </c>
+      <c r="T13" s="39">
+        <v>0</v>
+      </c>
+      <c r="U13" s="41">
+        <v>0</v>
+      </c>
+      <c r="V13" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13" s="33">
+        <f ca="1"/>
+        <v>9.9999999999999991E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="35">
+        <v>1.7189599999999999E-2</v>
+      </c>
+      <c r="D14" s="43">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="24">
+        <f ca="1"/>
+        <v>1.7189599999999999E-2</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="36">
+        <v>1.70896E-2</v>
+      </c>
+      <c r="I14" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="K14" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="38">
+        <v>0</v>
+      </c>
+      <c r="M14" s="39">
+        <v>0</v>
+      </c>
+      <c r="N14" s="39">
+        <v>0</v>
+      </c>
+      <c r="O14" s="39">
+        <v>0</v>
+      </c>
+      <c r="P14" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="48">
+        <v>1</v>
+      </c>
+      <c r="R14" s="49">
+        <v>0</v>
+      </c>
+      <c r="S14" s="49">
+        <v>0</v>
+      </c>
+      <c r="T14" s="49">
+        <v>0</v>
+      </c>
+      <c r="U14" s="50">
+        <v>0</v>
+      </c>
+      <c r="V14" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="W14" s="33">
+        <f ca="1"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="35">
+        <v>1.4835764423811048E-2</v>
+      </c>
+      <c r="D15" s="43">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1837587804604255E-7</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="24">
+        <f ca="1"/>
+        <v>1.4835882799689094E-2</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="36">
+        <v>1.4735882799689095E-2</v>
+      </c>
+      <c r="I15" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="K15" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" s="38">
+        <v>0</v>
+      </c>
+      <c r="M15" s="39">
+        <v>0</v>
+      </c>
+      <c r="N15" s="39">
+        <v>0</v>
+      </c>
+      <c r="O15" s="39">
+        <v>0</v>
+      </c>
+      <c r="P15" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="51">
+        <v>-1.013100581860171</v>
+      </c>
+      <c r="R15" s="39">
+        <v>2.0131005818601713</v>
+      </c>
+      <c r="S15" s="39">
+        <v>0</v>
+      </c>
+      <c r="T15" s="39">
+        <v>0</v>
+      </c>
+      <c r="U15" s="41">
+        <v>0</v>
+      </c>
+      <c r="V15" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="W15" s="33">
+        <f ca="1"/>
+        <v>1.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="35">
+        <v>1.5052961492011142E-2</v>
+      </c>
+      <c r="D16" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.7474789956600305E-8</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="24">
+        <f ca="1"/>
+        <v>1.5053058966801099E-2</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="36">
+        <v>1.4953058966801099E-2</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="K16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" s="38">
+        <v>0</v>
+      </c>
+      <c r="M16" s="39">
+        <v>0</v>
+      </c>
+      <c r="N16" s="39">
+        <v>0</v>
+      </c>
+      <c r="O16" s="39">
+        <v>0</v>
+      </c>
+      <c r="P16" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="51">
+        <v>1.6865017081063214E-16</v>
+      </c>
+      <c r="R16" s="39">
+        <v>-2.0381313856749337</v>
+      </c>
+      <c r="S16" s="39">
+        <v>3.0381313856749337</v>
+      </c>
+      <c r="T16" s="39">
+        <v>0</v>
+      </c>
+      <c r="U16" s="41">
+        <v>0</v>
+      </c>
+      <c r="V16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="W16" s="33">
+        <f ca="1"/>
+        <v>1.0000000000000002E-4</v>
+      </c>
+      <c r="AC16" s="60"/>
+    </row>
+    <row r="17" spans="2:23" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="35">
+        <v>1.5693437006418908E-2</v>
+      </c>
+      <c r="D17" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2969961285524967E-9</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="24">
+        <f ca="1"/>
+        <v>1.5693438303415037E-2</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="36">
+        <v>1.5593438303415037E-2</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="K17" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="38">
+        <v>0</v>
+      </c>
+      <c r="M17" s="39">
+        <v>0</v>
+      </c>
+      <c r="N17" s="39">
+        <v>0</v>
+      </c>
+      <c r="O17" s="39">
+        <v>0</v>
+      </c>
+      <c r="P17" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="51">
+        <v>5.5511151231257852E-17</v>
+      </c>
+      <c r="R17" s="39">
+        <v>0</v>
+      </c>
+      <c r="S17" s="39">
+        <v>-3.0769983737932272</v>
+      </c>
+      <c r="T17" s="39">
+        <v>4.0769983737932272</v>
+      </c>
+      <c r="U17" s="41">
+        <v>0</v>
+      </c>
+      <c r="V17" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="W17" s="33">
+        <f ca="1"/>
+        <v>1.0000000000000005E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="52">
+        <v>1.6399994544683334E-2</v>
+      </c>
+      <c r="D18" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1.4177239140988895E-7</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="25">
+        <f ca="1"/>
+        <v>1.6399852772291924E-2</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="53">
+        <v>1.6299852772291925E-2</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="54">
+        <v>1E-4</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="L18" s="55">
+        <v>0</v>
+      </c>
+      <c r="M18" s="56">
+        <v>0</v>
+      </c>
+      <c r="N18" s="56">
+        <v>0</v>
+      </c>
+      <c r="O18" s="56">
+        <v>0</v>
+      </c>
+      <c r="P18" s="56">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="57">
+        <v>-2.2935090300213447E-16</v>
+      </c>
+      <c r="R18" s="56">
+        <v>5.697241084667845E-16</v>
+      </c>
+      <c r="S18" s="56">
+        <v>-5.697241084667845E-16</v>
+      </c>
+      <c r="T18" s="56">
+        <v>-4.1316185651899975</v>
+      </c>
+      <c r="U18" s="58">
+        <v>5.1316185651899975</v>
+      </c>
+      <c r="V18" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="W18" s="34">
+        <f ca="1"/>
+        <v>9.9999999999999991E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="J20" s="59"/>
+      <c r="L20" s="63" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" ht="37.5" x14ac:dyDescent="0.5">
+      <c r="L21" s="64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B24" s="14"/>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B28" s="61"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J373"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1158,7 +4408,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="10">
-        <f ca="1">EXP(-rate*(C8-B8))</f>
+        <f t="shared" ref="D8:D37" ca="1" si="0">EXP(-rate*(C8-B8))</f>
         <v>1</v>
       </c>
       <c r="E8" s="8" t="e">
@@ -1176,11 +4426,11 @@
         <v>0</v>
       </c>
       <c r="C9" s="4">
-        <f ca="1">C8+dt</f>
+        <f t="shared" ref="C9:C37" ca="1" si="1">C8+dt</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D9" s="10">
-        <f ca="1">EXP(-rate*(C9-B9))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99916701379245831</v>
       </c>
       <c r="E9" s="6">
@@ -1198,19 +4448,19 @@
         <v>0</v>
       </c>
       <c r="C10" s="4">
-        <f ca="1">C9+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="D10" s="10">
-        <f ca="1">EXP(-rate*(C10-B10))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99833472145093871</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" ref="E10:E37" ca="1" si="0">-LN(D10)/(C10-B10)</f>
+        <f t="shared" ref="E10:E37" ca="1" si="2">-LN(D10)/(C10-B10)</f>
         <v>9.9999999999998059E-3</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" ref="F10:F37" ca="1" si="1">E10+G10</f>
+        <f t="shared" ref="F10:F37" ca="1" si="3">E10+G10</f>
         <v>9.9999999999998059E-3</v>
       </c>
       <c r="G10" s="11"/>
@@ -1220,19 +4470,19 @@
         <v>0</v>
       </c>
       <c r="C11" s="4">
-        <f ca="1">C10+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.25</v>
       </c>
       <c r="D11" s="10">
-        <f ca="1">EXP(-rate*(C11-B11))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99750312239746008</v>
       </c>
       <c r="E11" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000158E-2</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>3.0000000000000158E-2</v>
       </c>
       <c r="G11" s="11">
@@ -1244,19 +4494,19 @@
         <v>0</v>
       </c>
       <c r="C12" s="4">
-        <f ca="1">C11+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="D12" s="10">
-        <f ca="1">EXP(-rate*(C12-B12))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99667221605452327</v>
       </c>
       <c r="E12" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000142E-2</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000142E-2</v>
       </c>
       <c r="G12" s="11"/>
@@ -1266,19 +4516,19 @@
         <v>0</v>
       </c>
       <c r="C13" s="4">
-        <f ca="1">C12+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.41666666666666663</v>
       </c>
       <c r="D13" s="10">
-        <f ca="1">EXP(-rate*(C13-B13))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99584200184510996</v>
       </c>
       <c r="E13" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999655E-3</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999655E-3</v>
       </c>
       <c r="G13" s="11"/>
@@ -1288,65 +4538,65 @@
         <v>0</v>
       </c>
       <c r="C14" s="4">
-        <f ca="1">C13+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.49999999999999994</v>
       </c>
       <c r="D14" s="10">
-        <f ca="1">EXP(-rate*(C14-B14))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99501247919268232</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999881E-3</v>
       </c>
       <c r="F14" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.7499999999999988E-2</v>
-      </c>
-      <c r="G14" s="11">
-        <v>7.4999999999999997E-3</v>
-      </c>
+        <f t="shared" ca="1" si="3"/>
+        <v>9.9999999999999881E-3</v>
+      </c>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>0</v>
       </c>
       <c r="C15" s="4">
-        <f ca="1">C14+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.58333333333333326</v>
       </c>
       <c r="D15" s="10">
-        <f ca="1">EXP(-rate*(C15-B15))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99418364752118304</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999204E-3</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.9999999999999204E-3</v>
-      </c>
-      <c r="G15" s="11"/>
+        <f t="shared" ca="1" si="3"/>
+        <v>1.7499999999999918E-2</v>
+      </c>
+      <c r="G15" s="11">
+        <v>7.4999999999999997E-3</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>0</v>
       </c>
       <c r="C16" s="4">
-        <f ca="1">C15+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D16" s="10">
-        <f ca="1">EXP(-rate*(C16-B16))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99335550625503444</v>
       </c>
       <c r="E16" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999672E-3</v>
       </c>
       <c r="F16" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999672E-3</v>
       </c>
       <c r="G16" s="11"/>
@@ -1356,43 +4606,41 @@
         <v>0</v>
       </c>
       <c r="C17" s="4">
-        <f ca="1">C16+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.75</v>
       </c>
       <c r="D17" s="10">
-        <f ca="1">EXP(-rate*(C17-B17))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99252805481913842</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000018E-2</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2500000000000018E-2</v>
-      </c>
-      <c r="G17" s="11">
-        <v>2.5000000000000001E-3</v>
-      </c>
+        <f t="shared" ca="1" si="3"/>
+        <v>1.0000000000000018E-2</v>
+      </c>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>0</v>
       </c>
       <c r="C18" s="4">
-        <f ca="1">C17+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="D18" s="10">
-        <f ca="1">EXP(-rate*(C18-B18))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99170129263887596</v>
       </c>
       <c r="E18" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999915E-3</v>
       </c>
       <c r="F18" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999915E-3</v>
       </c>
       <c r="G18" s="11"/>
@@ -1402,41 +4650,43 @@
         <v>0</v>
       </c>
       <c r="C19" s="4">
-        <f ca="1">C18+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.91666666666666674</v>
       </c>
       <c r="D19" s="10">
-        <f ca="1">EXP(-rate*(C19-B19))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99087521914010657</v>
       </c>
       <c r="E19" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999915E-3</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.9999999999999915E-3</v>
-      </c>
-      <c r="G19" s="11"/>
+        <f t="shared" ca="1" si="3"/>
+        <v>1.2499999999999992E-2</v>
+      </c>
+      <c r="G19" s="11">
+        <v>2.5000000000000001E-3</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>0</v>
       </c>
       <c r="C20" s="4">
-        <f ca="1">C19+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D20" s="10">
-        <f ca="1">EXP(-rate*(C20-B20))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.99004983374916811</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999464E-3</v>
       </c>
       <c r="F20" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999464E-3</v>
       </c>
       <c r="G20" s="11"/>
@@ -1446,19 +4696,19 @@
         <v>0</v>
       </c>
       <c r="C21" s="4">
-        <f ca="1">C20+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.0833333333333333</v>
       </c>
       <c r="D21" s="10">
-        <f ca="1">EXP(-rate*(C21-B21))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98922513589287608</v>
       </c>
       <c r="E21" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000021E-2</v>
       </c>
       <c r="F21" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000021E-2</v>
       </c>
       <c r="G21" s="11"/>
@@ -1468,19 +4718,19 @@
         <v>0</v>
       </c>
       <c r="C22" s="4">
-        <f ca="1">C21+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.1666666666666665</v>
       </c>
       <c r="D22" s="10">
-        <f ca="1">EXP(-rate*(C22-B22))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98840112499852384</v>
       </c>
       <c r="E22" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999985E-3</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999985E-3</v>
       </c>
       <c r="G22" s="11"/>
@@ -1490,19 +4740,19 @@
         <v>0</v>
       </c>
       <c r="C23" s="4">
-        <f ca="1">C22+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.2499999999999998</v>
       </c>
       <c r="D23" s="10">
-        <f ca="1">EXP(-rate*(C23-B23))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98757780049388144</v>
       </c>
       <c r="E23" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999915E-3</v>
       </c>
       <c r="F23" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999915E-3</v>
       </c>
       <c r="G23" s="11"/>
@@ -1512,19 +4762,19 @@
         <v>0</v>
       </c>
       <c r="C24" s="4">
-        <f ca="1">C23+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.333333333333333</v>
       </c>
       <c r="D24" s="10">
-        <f ca="1">EXP(-rate*(C24-B24))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98675516180719569</v>
       </c>
       <c r="E24" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000023E-2</v>
       </c>
       <c r="F24" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000023E-2</v>
       </c>
       <c r="G24" s="11"/>
@@ -1534,19 +4784,19 @@
         <v>0</v>
       </c>
       <c r="C25" s="4">
-        <f ca="1">C24+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.4166666666666663</v>
       </c>
       <c r="D25" s="10">
-        <f ca="1">EXP(-rate*(C25-B25))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98593320836718978</v>
       </c>
       <c r="E25" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000019E-2</v>
       </c>
       <c r="F25" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000019E-2</v>
       </c>
       <c r="G25" s="11"/>
@@ -1556,19 +4806,19 @@
         <v>0</v>
       </c>
       <c r="C26" s="4">
-        <f ca="1">C25+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.4999999999999996</v>
       </c>
       <c r="D26" s="10">
-        <f ca="1">EXP(-rate*(C26-B26))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98511193960306265</v>
       </c>
       <c r="E26" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000012E-2</v>
       </c>
       <c r="F26" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000012E-2</v>
       </c>
       <c r="G26" s="11"/>
@@ -1578,19 +4828,19 @@
         <v>0</v>
       </c>
       <c r="C27" s="4">
-        <f ca="1">C26+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.5833333333333328</v>
       </c>
       <c r="D27" s="10">
-        <f ca="1">EXP(-rate*(C27-B27))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98429135494448872</v>
       </c>
       <c r="E27" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000004E-2</v>
       </c>
       <c r="F27" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000004E-2</v>
       </c>
       <c r="G27" s="11"/>
@@ -1600,19 +4850,19 @@
         <v>0</v>
       </c>
       <c r="C28" s="4">
-        <f ca="1">C27+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.6666666666666661</v>
       </c>
       <c r="D28" s="10">
-        <f ca="1">EXP(-rate*(C28-B28))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98347145382161749</v>
       </c>
       <c r="E28" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="F28" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="G28" s="11"/>
@@ -1622,19 +4872,19 @@
         <v>0</v>
       </c>
       <c r="C29" s="4">
-        <f ca="1">C28+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.7499999999999993</v>
       </c>
       <c r="D29" s="10">
-        <f ca="1">EXP(-rate*(C29-B29))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.9826522356650732</v>
       </c>
       <c r="E29" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999777E-3</v>
       </c>
       <c r="F29" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999777E-3</v>
       </c>
       <c r="G29" s="11"/>
@@ -1644,19 +4894,19 @@
         <v>0</v>
       </c>
       <c r="C30" s="4">
-        <f ca="1">C29+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.8333333333333326</v>
       </c>
       <c r="D30" s="10">
-        <f ca="1">EXP(-rate*(C30-B30))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98183369990595426</v>
       </c>
       <c r="E30" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999707E-3</v>
       </c>
       <c r="F30" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999707E-3</v>
       </c>
       <c r="G30" s="11"/>
@@ -1666,19 +4916,19 @@
         <v>0</v>
       </c>
       <c r="C31" s="4">
-        <f ca="1">C30+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.9166666666666659</v>
       </c>
       <c r="D31" s="10">
-        <f ca="1">EXP(-rate*(C31-B31))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98101584597583302</v>
       </c>
       <c r="E31" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999725E-3</v>
       </c>
       <c r="F31" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999725E-3</v>
       </c>
       <c r="G31" s="11"/>
@@ -1688,19 +4938,19 @@
         <v>0</v>
       </c>
       <c r="C32" s="4">
-        <f ca="1">C31+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.9999999999999991</v>
       </c>
       <c r="D32" s="10">
-        <f ca="1">EXP(-rate*(C32-B32))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.98019867330675536</v>
       </c>
       <c r="E32" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999742E-3</v>
       </c>
       <c r="F32" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999742E-3</v>
       </c>
       <c r="G32" s="11"/>
@@ -1710,19 +4960,19 @@
         <v>0</v>
       </c>
       <c r="C33" s="4">
-        <f ca="1">C32+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2.0833333333333326</v>
       </c>
       <c r="D33" s="10">
-        <f ca="1">EXP(-rate*(C33-B33))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.97938218133124022</v>
       </c>
       <c r="E33" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999759E-3</v>
       </c>
       <c r="F33" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999759E-3</v>
       </c>
       <c r="G33" s="11"/>
@@ -1732,19 +4982,19 @@
         <v>0</v>
       </c>
       <c r="C34" s="4">
-        <f ca="1">C33+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2.1666666666666661</v>
       </c>
       <c r="D34" s="10">
-        <f ca="1">EXP(-rate*(C34-B34))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.97856636948227915</v>
       </c>
       <c r="E34" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000024E-2</v>
       </c>
       <c r="F34" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000024E-2</v>
       </c>
       <c r="G34" s="11"/>
@@ -1754,19 +5004,19 @@
         <v>0</v>
       </c>
       <c r="C35" s="4">
-        <f ca="1">C34+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2.2499999999999996</v>
       </c>
       <c r="D35" s="10">
-        <f ca="1">EXP(-rate*(C35-B35))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.97775123719333634</v>
       </c>
       <c r="E35" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000012E-2</v>
       </c>
       <c r="F35" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000012E-2</v>
       </c>
       <c r="G35" s="11"/>
@@ -1776,19 +5026,19 @@
         <v>0</v>
       </c>
       <c r="C36" s="4">
-        <f ca="1">C35+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2.333333333333333</v>
       </c>
       <c r="D36" s="10">
-        <f ca="1">EXP(-rate*(C36-B36))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.97693678389834759</v>
       </c>
       <c r="E36" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9999999999999777E-3</v>
       </c>
       <c r="F36" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>9.9999999999999777E-3</v>
       </c>
       <c r="G36" s="11"/>
@@ -1798,19 +5048,19 @@
         <v>0</v>
       </c>
       <c r="C37" s="4">
-        <f ca="1">C36+dt</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2.4166666666666665</v>
       </c>
       <c r="D37" s="10">
-        <f ca="1">EXP(-rate*(C37-B37))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.97612300903172011</v>
       </c>
       <c r="E37" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="F37" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="G37" s="11"/>
@@ -4508,28 +7758,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>